<commit_message>
I added player statisitcs to each contract file. In the main file I added links, metrics, helpful info and wrote down info that I researched as well
</commit_message>
<xml_diff>
--- a/Contracts/NBA and WNBA Contracts 2019-2023 (2).xlsx
+++ b/Contracts/NBA and WNBA Contracts 2019-2023 (2).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99ba0c85aecb9b53/Desktop/Contracts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanm\smu\NBA-VS-WNBA\Contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26C70F26-ACB0-4047-AEEE-A1C7EA568F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B978A2-C9D3-4B7C-BE8C-115BC05E637C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{56C3912B-2DA3-43BE-93F2-97F2E0B2F679}"/>
   </bookViews>
@@ -17,23 +17,25 @@
     <sheet name="NBA 2020-2021" sheetId="3" r:id="rId2"/>
     <sheet name="NBA 2021-2022 " sheetId="4" r:id="rId3"/>
     <sheet name="NBA 2022-2023" sheetId="5" r:id="rId4"/>
-    <sheet name="WNBA" sheetId="2" r:id="rId5"/>
-    <sheet name="WNBA 2019" sheetId="11" r:id="rId6"/>
-    <sheet name="WNBA 2020" sheetId="6" r:id="rId7"/>
-    <sheet name="WNBA 2021" sheetId="7" r:id="rId8"/>
-    <sheet name="WNBA 2022" sheetId="8" r:id="rId9"/>
-    <sheet name="WNBA 2023" sheetId="9" r:id="rId10"/>
+    <sheet name="NBA Cap" sheetId="13" r:id="rId5"/>
+    <sheet name="WNBA" sheetId="2" r:id="rId6"/>
+    <sheet name="WNBA 2019" sheetId="11" r:id="rId7"/>
+    <sheet name="WNBA 2020" sheetId="6" r:id="rId8"/>
+    <sheet name="WNBA 2021" sheetId="7" r:id="rId9"/>
+    <sheet name="WNBA 2022" sheetId="8" r:id="rId10"/>
+    <sheet name="WNBA 2023" sheetId="9" r:id="rId11"/>
+    <sheet name="WNBA Cap" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NBA!$C$53:$C$205</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NBA 2020-2021'!$A$3:$E$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'NBA 2021-2022 '!$A$1:$E$2772</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'NBA 2022-2023'!$A$1:$F$523</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'WNBA 2019'!$A$3:$B$159</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'WNBA 2020'!$A$1:$F$679</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'WNBA 2021'!$A$1:$F$616</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'WNBA 2022'!$A$1:$F$616</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'WNBA 2023'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'WNBA 2019'!$A$3:$B$159</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'WNBA 2020'!$A$1:$F$679</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'WNBA 2021'!$A$1:$F$616</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'WNBA 2022'!$A$1:$F$616</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'WNBA 2023'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3665" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="351">
   <si>
     <t>2019-2020</t>
   </si>
@@ -859,15 +861,256 @@
   <si>
     <t>WAS</t>
   </si>
+  <si>
+    <t>WNBA CBA and Salary Cap Explained | Statistics, Ranks, Game Logs and more Women's Basketball Insight from Her Hoop Stats</t>
+  </si>
+  <si>
+    <t>Salary Cap</t>
+  </si>
+  <si>
+    <t>What are the salary cap and team minimum?</t>
+  </si>
+  <si>
+    <t>The salary cap is the maximum allowed total salary of all the players a team has on the books. The WNBA is different from most other professional sports leagues in the US in that the salary cap is a hard cap with very little wiggle room. The only way that a team can go above the salary cap during the regular season is if the league has granted them hardship or emergency hardship exceptions.</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>Under the latest CBA, the salary cap is specified for each season through 2027 with annual increases of 3% each season. The minimum team salary level increases at the same rate. With a few exceptions, this is about in line with the maximum increase a contract can see in each season. The minimum team salary, which works out to be 83.7% of the salary cap, is the minimum total salary a team may have by the end of each season. Teams may be below the minimum before the season and throughout the season with no penalty.</t>
+  </si>
+  <si>
+    <t>WNBA Salary Cap 2023: What You Need to Know - Boardroom</t>
+  </si>
+  <si>
+    <t>WNBA's new labor deal hikes average salary to $130,000, provides paid maternity leave - CBS News</t>
+  </si>
+  <si>
+    <t>2019-2023 Min Vet salary</t>
+  </si>
+  <si>
+    <t>2019-2023 Max Vet salary</t>
+  </si>
+  <si>
+    <t>2019-2023 Min Rookie salary</t>
+  </si>
+  <si>
+    <t>2019-2023 Max Rookie salary</t>
+  </si>
+  <si>
+    <t>WNBA news: Takeaways from the WNBA salary database (highposthoops.com)</t>
+  </si>
+  <si>
+    <t>2023 NBA salary cap tracker by team: From healthy to disastrous (sportsnaut.com)</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>0-6 Years of Experience</t>
+  </si>
+  <si>
+    <t>7-9 Years of Experience</t>
+  </si>
+  <si>
+    <t>10+ Years of Experience</t>
+  </si>
+  <si>
+    <t>1 Years of Experience</t>
+  </si>
+  <si>
+    <t>0 Years of Experience</t>
+  </si>
+  <si>
+    <t>2 Years of Experience</t>
+  </si>
+  <si>
+    <t>Team Salary Cap</t>
+  </si>
+  <si>
+    <t>NBA Minimum Salaries For 2023/24 | Hoops Rumors</t>
+  </si>
+  <si>
+    <t>Salary cap set at $112.4 million for 2021-22 season | NBA.com</t>
+  </si>
+  <si>
+    <t>The salary cap for the 2022–23 season is $123.655 million (minimum team salary, which is set at 90 percent of the Salary Cap, is $111.290 million)</t>
+  </si>
+  <si>
+    <t>NBA Salary Cap set at $109.14 million for 2019-20 | NBA.com</t>
+  </si>
+  <si>
+    <t>What is the minimum salary for a 10 day NBA contract?</t>
+  </si>
+  <si>
+    <t>2023 NBA 10-day contract explained: How it works and salary limits | Marca</t>
+  </si>
+  <si>
+    <t>$62,285 </t>
+  </si>
+  <si>
+    <t>Minimum base salary for a 7 day contract is:</t>
+  </si>
+  <si>
+    <t>The average career is only 3½ years</t>
+  </si>
+  <si>
+    <t>Throughout NBA history there have been more than 4,400 players, and the average career length is around 4.5 years.</t>
+  </si>
+  <si>
+    <t>Retirement is around 35 years old</t>
+  </si>
+  <si>
+    <t>Most players are between the ages of 20 and 25 during their first NBA season</t>
+  </si>
+  <si>
+    <t>What is the average age in the WNBA?</t>
+  </si>
+  <si>
+    <t>The average age over the history of the league is 27.3.</t>
+  </si>
+  <si>
+    <t>How long is the average WNBA players career?</t>
+  </si>
+  <si>
+    <t>Roughly 3.5 to 5 years</t>
+  </si>
+  <si>
+    <t>$61,000 to $175,000 dollars</t>
+  </si>
+  <si>
+    <t>(CBA 2019)</t>
+  </si>
+  <si>
+    <t>WNBA</t>
+  </si>
+  <si>
+    <t>Min Base Salary</t>
+  </si>
+  <si>
+    <t>Max Base Salary</t>
+  </si>
+  <si>
+    <t>Minimum Team Salary (90%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM SALARY CAP (3%+) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINIMUM TEAM SALARY  (3%+) </t>
+  </si>
+  <si>
+    <t>NBA</t>
+  </si>
+  <si>
+    <t>Uniform Player contract</t>
+  </si>
+  <si>
+    <t>Max contract</t>
+  </si>
+  <si>
+    <t>Supermax contract</t>
+  </si>
+  <si>
+    <t>Rookie scale contract</t>
+  </si>
+  <si>
+    <t>Designate Veteran Player Contract</t>
+  </si>
+  <si>
+    <t>Two-Way Contract</t>
+  </si>
+  <si>
+    <t>Summer Contract</t>
+  </si>
+  <si>
+    <t>Non-Guaranteed Training Camp Contract</t>
+  </si>
+  <si>
+    <t>Exhibit 10</t>
+  </si>
+  <si>
+    <t>10 day contract</t>
+  </si>
+  <si>
+    <t>Rest of Season contract</t>
+  </si>
+  <si>
+    <t>Top 5 Rookie season contracts for 2023</t>
+  </si>
+  <si>
+    <t>Victor Wembanyama $12,200,000</t>
+  </si>
+  <si>
+    <t>Brandon Miller $10,900,000</t>
+  </si>
+  <si>
+    <t>Scoot Henderson $9,800,000</t>
+  </si>
+  <si>
+    <t>Amen Thompson $8,800,000</t>
+  </si>
+  <si>
+    <t>Ausar Thompson $8,000,000</t>
+  </si>
+  <si>
+    <t>Aliyah Boston $74,305</t>
+  </si>
+  <si>
+    <t>Diamond Miller $74,305</t>
+  </si>
+  <si>
+    <t>Maddy Siegrist $74,305</t>
+  </si>
+  <si>
+    <t>Stephanie Soares $74,305</t>
+  </si>
+  <si>
+    <t>Lou Lopez Sénéchal $71,300</t>
+  </si>
+  <si>
+    <t>Top 5 Max contracts for 2022-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephen Curry $48,070,014                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LeBron James $44,474,988 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Durant $44,119,845 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bradley Beal $43,279,250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damian Lillard $42,492,492 </t>
+  </si>
+  <si>
+    <t>Jewell Loyd $234,936</t>
+  </si>
+  <si>
+    <t>Arike Ogunbowale $234,936</t>
+  </si>
+  <si>
+    <t>Diana Taurasi $234,936</t>
+  </si>
+  <si>
+    <t>DeWanna Bonner $234,350</t>
+  </si>
+  <si>
+    <t>Elena Delle Donne $234,350</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -933,16 +1176,100 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -950,12 +1277,117 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1005,6 +1437,103 @@
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1336,7 +1865,7 @@
   <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5955,6 +6484,1205 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE39DD43-5148-45D7-9D36-7E25A97CBC50}">
+  <dimension ref="A1:L51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.4140625" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.9140625" customWidth="1"/>
+    <col min="9" max="9" width="19.58203125" customWidth="1"/>
+    <col min="13" max="13" width="21.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="8">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="16">
+        <v>228094</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="8">
+        <v>40</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="16">
+        <v>228094</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="8">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="16">
+        <v>228094</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8">
+        <v>31</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="16">
+        <v>227900</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8">
+        <v>34</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="16">
+        <v>227900</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="16">
+        <v>227900</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="8">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="16">
+        <v>227900</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8">
+        <v>30</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="16">
+        <v>221450</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="8">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="16">
+        <v>215000</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="8">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="16">
+        <v>206267</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8">
+        <v>30</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="16">
+        <v>206000</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8">
+        <v>28</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="16">
+        <v>205000</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="8">
+        <v>27</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="16">
+        <v>200000</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="8">
+        <v>26</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="16">
+        <v>200000</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8">
+        <v>36</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="16">
+        <v>200000</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="8">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="16">
+        <v>196267</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="8">
+        <v>26</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="16">
+        <v>196267</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="8">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="16">
+        <v>196267</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="8">
+        <v>30</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="16">
+        <v>196267</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="8">
+        <v>32</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="16">
+        <v>196267</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="8">
+        <v>35</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="16">
+        <v>196100</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="12"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="8">
+        <v>36</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="16">
+        <v>195000</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="8">
+        <v>33</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="16">
+        <v>195000</v>
+      </c>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="8">
+        <v>29</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="16">
+        <v>190550</v>
+      </c>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="12"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="8">
+        <v>32</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="16">
+        <v>190000</v>
+      </c>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="8">
+        <v>31</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="16">
+        <v>185400</v>
+      </c>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="12"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="8">
+        <v>29</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="16">
+        <v>185000</v>
+      </c>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="12"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="8">
+        <v>30</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="16">
+        <v>185000</v>
+      </c>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="8">
+        <v>35</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="16">
+        <v>183000</v>
+      </c>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="8">
+        <v>27</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="16">
+        <v>180250</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="12"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="8">
+        <v>26</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="16">
+        <v>170000</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="12"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="8">
+        <v>26</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="16">
+        <v>170000</v>
+      </c>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="12"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="8">
+        <v>27</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="16">
+        <v>164800</v>
+      </c>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="12"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="8">
+        <v>27</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F35" s="16">
+        <v>160000</v>
+      </c>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="12"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="8">
+        <v>29</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="16">
+        <v>160000</v>
+      </c>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="12"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="8">
+        <v>30</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="16">
+        <v>160000</v>
+      </c>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="12"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="8">
+        <v>28</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="16">
+        <v>159000</v>
+      </c>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="8">
+        <v>33</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" s="16">
+        <v>155000</v>
+      </c>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="12"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="8">
+        <v>28</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" s="16">
+        <v>152800</v>
+      </c>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="12"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="8">
+        <v>34</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="16">
+        <v>150350</v>
+      </c>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="12"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="8">
+        <v>27</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="16">
+        <v>150000</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="8">
+        <v>27</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" s="16">
+        <v>148400</v>
+      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="12"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="8">
+        <v>32</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="16">
+        <v>145000</v>
+      </c>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="12"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="8">
+        <v>25</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="16">
+        <v>144000</v>
+      </c>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="8">
+        <v>29</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F46" s="16">
+        <v>141000</v>
+      </c>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="12"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="8">
+        <v>26</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" s="16">
+        <v>140000</v>
+      </c>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="8">
+        <v>35</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="16">
+        <v>140000</v>
+      </c>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="12"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="8">
+        <v>26</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F49" s="16">
+        <v>140000</v>
+      </c>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="12"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="8">
+        <v>28</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="16">
+        <v>139000</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="8">
+        <v>36</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F51" s="16">
+        <v>135000</v>
+      </c>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="12"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F51">
+    <sortCondition descending="1" ref="F2:F51"/>
+  </sortState>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73831D4F-A766-43CC-BECD-F962438B1DED}">
   <dimension ref="A1:L52"/>
   <sheetViews>
@@ -7168,6 +8896,347 @@
     <sortCondition descending="1" ref="F2:F51"/>
   </sortState>
   <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4995DF26-E1FD-4687-82B0-E0A0D35DBBB7}">
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="24.4140625" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="7" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>300</v>
+      </c>
+      <c r="C11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:8" ht="25" x14ac:dyDescent="0.5">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="40" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="23">
+        <v>2019</v>
+      </c>
+      <c r="B18" s="24">
+        <v>996100</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="D18" s="24">
+        <v>117500</v>
+      </c>
+      <c r="E18" s="24">
+        <v>53000</v>
+      </c>
+      <c r="F18" s="24">
+        <v>115000</v>
+      </c>
+      <c r="G18" s="24">
+        <v>41965</v>
+      </c>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="23">
+        <v>2020</v>
+      </c>
+      <c r="B19" s="24">
+        <v>1300000</v>
+      </c>
+      <c r="C19" s="24">
+        <v>1088100</v>
+      </c>
+      <c r="D19" s="24">
+        <v>215000</v>
+      </c>
+      <c r="E19" s="24">
+        <v>68000</v>
+      </c>
+      <c r="F19" s="24">
+        <v>185000</v>
+      </c>
+      <c r="G19" s="24">
+        <v>57000</v>
+      </c>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="23">
+        <v>2021</v>
+      </c>
+      <c r="B20" s="24">
+        <v>1339000</v>
+      </c>
+      <c r="C20" s="24">
+        <v>1120770</v>
+      </c>
+      <c r="D20" s="24">
+        <v>221450</v>
+      </c>
+      <c r="E20" s="24">
+        <v>70000</v>
+      </c>
+      <c r="F20" s="24">
+        <v>190500</v>
+      </c>
+      <c r="G20" s="24">
+        <v>59000</v>
+      </c>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="23">
+        <v>2022</v>
+      </c>
+      <c r="B21" s="24">
+        <v>1379200</v>
+      </c>
+      <c r="C21" s="24">
+        <v>1154340</v>
+      </c>
+      <c r="D21" s="24">
+        <v>228094</v>
+      </c>
+      <c r="E21" s="24">
+        <v>72000</v>
+      </c>
+      <c r="F21" s="24">
+        <v>196267</v>
+      </c>
+      <c r="G21" s="24">
+        <v>60000</v>
+      </c>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="23">
+        <v>2023</v>
+      </c>
+      <c r="B22" s="24">
+        <v>1420500</v>
+      </c>
+      <c r="C22" s="24">
+        <v>1188990</v>
+      </c>
+      <c r="D22" s="25">
+        <v>234936</v>
+      </c>
+      <c r="E22" s="24">
+        <v>74000</v>
+      </c>
+      <c r="F22" s="25">
+        <v>202154</v>
+      </c>
+      <c r="G22" s="24">
+        <v>62000</v>
+      </c>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="23">
+        <v>2024</v>
+      </c>
+      <c r="B23" s="24">
+        <v>1463200</v>
+      </c>
+      <c r="C23" s="24">
+        <v>1224630</v>
+      </c>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="23">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="24">
+        <v>1507100</v>
+      </c>
+      <c r="C24" s="24">
+        <v>1261440</v>
+      </c>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="23">
+        <v>2026</v>
+      </c>
+      <c r="B25" s="24">
+        <v>1552300</v>
+      </c>
+      <c r="C25" s="24">
+        <v>1299240</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="23">
+        <v>2027</v>
+      </c>
+      <c r="B26" s="24">
+        <v>1598800</v>
+      </c>
+      <c r="C26" s="24">
+        <v>1338210</v>
+      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="salary_cap" display="https://herhoopstats.com/wnba_cba_salary_cap_explained - salary_cap" xr:uid="{0943F386-15D6-4989-9B6C-C59BD3540441}"/>
+    <hyperlink ref="A2" r:id="rId2" location=":~:text=Inside%20the%20WNBA%20Salary%20Cap%20for%202023&amp;text=That%27s%20up%20from%20%241%2C300%2C000%20in,year%20of%20the%20prior%20agreement." display="https://boardroom.tv/wnba-salary-cap-2023-max-salary/ - :~:text=Inside%20the%20WNBA%20Salary%20Cap%20for%202023&amp;text=That%27s%20up%20from%20%241%2C300%2C000%20in,year%20of%20the%20prior%20agreement." xr:uid="{A7EBA24F-61C9-40A1-9E8A-6F38461F41F3}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://highposthoops.com/2019/05/07/takeaways-from-wnba-salary-database/" xr:uid="{756CE5D2-58D9-4A2C-B20A-BB1A0FA0BAA2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -27083,10 +29152,668 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9128B9-7CCA-4DCB-96AC-92F522460BE8}">
+  <dimension ref="A1:I63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="22.25" customWidth="1"/>
+    <col min="3" max="3" width="28.58203125" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="36.4140625" customWidth="1"/>
+    <col min="6" max="6" width="32.08203125" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="38"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" ht="22" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="27"/>
+      <c r="B15" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
+      <c r="B16" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="33">
+        <v>109140000</v>
+      </c>
+      <c r="D16" s="33">
+        <v>98226000</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="33">
+        <v>109140000</v>
+      </c>
+      <c r="D17" s="33">
+        <v>98226000</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
+      <c r="B18" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="35">
+        <v>112414000</v>
+      </c>
+      <c r="D18" s="35">
+        <v>101173000</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="35">
+        <v>123655000</v>
+      </c>
+      <c r="D19" s="35">
+        <v>111290000</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="21"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="21"/>
+      <c r="B22" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="21"/>
+      <c r="B23" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="35">
+        <v>838464</v>
+      </c>
+      <c r="D23" s="35">
+        <v>1349383</v>
+      </c>
+      <c r="E23" s="35">
+        <v>1512601</v>
+      </c>
+      <c r="F23" s="35">
+        <v>2393887</v>
+      </c>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="21"/>
+      <c r="B24" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="35">
+        <v>898310</v>
+      </c>
+      <c r="D24" s="35">
+        <v>1445697</v>
+      </c>
+      <c r="E24" s="35">
+        <v>1620564</v>
+      </c>
+      <c r="F24" s="35">
+        <v>2564753</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="21"/>
+      <c r="B25" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="35">
+        <v>925258</v>
+      </c>
+      <c r="D25" s="35">
+        <v>1489065</v>
+      </c>
+      <c r="E25" s="35">
+        <v>1669178</v>
+      </c>
+      <c r="F25" s="35">
+        <v>2641691</v>
+      </c>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="21"/>
+      <c r="B26" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="35">
+        <v>1017781</v>
+      </c>
+      <c r="D26" s="35">
+        <v>1637966</v>
+      </c>
+      <c r="E26" s="35">
+        <v>1836090</v>
+      </c>
+      <c r="F26" s="35">
+        <v>2905851</v>
+      </c>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="21"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="21"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="F28" s="34"/>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+      <c r="B29" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="F29" s="34"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="21"/>
+      <c r="B30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="35">
+        <v>25467250</v>
+      </c>
+      <c r="D30" s="35">
+        <v>30560700</v>
+      </c>
+      <c r="E30" s="35">
+        <v>35654150</v>
+      </c>
+      <c r="F30" s="34"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="21"/>
+      <c r="B31" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="35">
+        <v>27285000</v>
+      </c>
+      <c r="D31" s="35">
+        <v>32742000</v>
+      </c>
+      <c r="E31" s="35">
+        <v>38199000</v>
+      </c>
+      <c r="F31" s="34"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="21"/>
+      <c r="B32" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="35">
+        <v>28103500</v>
+      </c>
+      <c r="D32" s="35">
+        <v>33724200</v>
+      </c>
+      <c r="E32" s="35">
+        <v>39344900</v>
+      </c>
+      <c r="F32" s="34"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="21"/>
+      <c r="B33" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="35">
+        <v>30913750</v>
+      </c>
+      <c r="D33" s="35">
+        <v>37096500</v>
+      </c>
+      <c r="E33" s="35">
+        <v>43279250</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D36" s="21"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>318</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="54" t="s">
+        <v>329</v>
+      </c>
+      <c r="F37" s="54"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="50"/>
+      <c r="E38" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="F38" s="52" t="s">
+        <v>335</v>
+      </c>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>320</v>
+      </c>
+      <c r="D39" s="21"/>
+      <c r="E39" s="49" t="s">
+        <v>331</v>
+      </c>
+      <c r="F39" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="G39" s="48"/>
+    </row>
+    <row r="40" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>321</v>
+      </c>
+      <c r="D40" s="21"/>
+      <c r="E40" s="49" t="s">
+        <v>332</v>
+      </c>
+      <c r="F40" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="G40" s="48"/>
+    </row>
+    <row r="41" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>322</v>
+      </c>
+      <c r="D41" s="50"/>
+      <c r="E41" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="F41" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="G41" s="48"/>
+    </row>
+    <row r="42" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>323</v>
+      </c>
+      <c r="D42" s="21"/>
+      <c r="E42" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="F42" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="G42" s="48"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>324</v>
+      </c>
+      <c r="D43" s="21"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="E49" s="41"/>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="E50" s="41"/>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D51" s="21"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="4:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="D52" s="50"/>
+      <c r="E52" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="F52" s="56"/>
+      <c r="G52" s="48"/>
+    </row>
+    <row r="53" spans="4:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="D53" s="50"/>
+      <c r="E53" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="F53" s="51" t="s">
+        <v>346</v>
+      </c>
+      <c r="G53" s="21"/>
+    </row>
+    <row r="54" spans="4:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="D54" s="50"/>
+      <c r="E54" s="58" t="s">
+        <v>342</v>
+      </c>
+      <c r="F54" s="52" t="s">
+        <v>347</v>
+      </c>
+      <c r="G54" s="48"/>
+    </row>
+    <row r="55" spans="4:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="D55" s="50"/>
+      <c r="E55" s="43" t="s">
+        <v>343</v>
+      </c>
+      <c r="F55" s="52" t="s">
+        <v>348</v>
+      </c>
+      <c r="G55" s="48"/>
+    </row>
+    <row r="56" spans="4:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="D56" s="50"/>
+      <c r="E56" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="F56" s="45" t="s">
+        <v>349</v>
+      </c>
+      <c r="G56" s="48"/>
+    </row>
+    <row r="57" spans="4:7" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="D57" s="50"/>
+      <c r="E57" s="43" t="s">
+        <v>345</v>
+      </c>
+      <c r="F57" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G57" s="48"/>
+    </row>
+    <row r="58" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="21"/>
+    </row>
+    <row r="63" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="E63" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E52:F52"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://sportsnaut.com/nba-salary-cap-tracker-team-by-team/" xr:uid="{377C2429-54D1-491D-B1CB-DEAE0E54F713}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://www.hoopsrumors.com/2023/07/nba-minimum-salaries-for-2023-24.html" xr:uid="{2D3173A1-49AD-41AD-8C98-41E8C718F597}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://www.nba.com/news/salary-cap-set-at-112-4-million-for-2021-22-season" xr:uid="{A74AB48C-9415-42B4-891B-6C52AEE40B5B}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://www.nba.com/news/nba-salary-cap-2019-20-season-set-10914-million" xr:uid="{04A4086D-F987-4BD5-AE5C-F36DBE183923}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.marca.com/en/basketball/nba/2023/01/04/63b5adaaca4741856d8b45c7.html" xr:uid="{1FAD3502-24DD-4CC6-830A-2442E6998BF9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A6E1F6-CE5B-4FF4-8052-5AE8624C24D7}">
   <dimension ref="A1:G258"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A247" workbookViewId="0">
       <selection activeCell="K188" sqref="K188"/>
     </sheetView>
   </sheetViews>
@@ -32978,11 +35705,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2874B52-658B-4860-B40F-3BBEBDFB2302}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -34094,7 +36821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5655F87D-9A0D-4F84-BDAD-3ADE9F5EE87F}">
   <dimension ref="A1:R51"/>
   <sheetViews>
@@ -35397,7 +38124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F558F5AB-8F6D-4F3E-9746-BF1CEFF80BBC}">
   <dimension ref="A1:L51"/>
   <sheetViews>
@@ -36594,1203 +39321,4 @@
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE39DD43-5148-45D7-9D36-7E25A97CBC50}">
-  <dimension ref="A1:L51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.4140625" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.9140625" customWidth="1"/>
-    <col min="9" max="9" width="19.58203125" customWidth="1"/>
-    <col min="13" max="13" width="21.58203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="8">
-        <v>27</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="16">
-        <v>228094</v>
-      </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="8">
-        <v>40</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="16">
-        <v>228094</v>
-      </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="8">
-        <v>28</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="16">
-        <v>228094</v>
-      </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="8">
-        <v>31</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F5" s="16">
-        <v>227900</v>
-      </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="8">
-        <v>34</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="16">
-        <v>227900</v>
-      </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="8">
-        <v>32</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="16">
-        <v>227900</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" s="8">
-        <v>32</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="16">
-        <v>227900</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="8">
-        <v>30</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="16">
-        <v>221450</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="8">
-        <v>32</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" s="16">
-        <v>215000</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="8">
-        <v>29</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F11" s="16">
-        <v>206267</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="8">
-        <v>30</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="16">
-        <v>206000</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="8">
-        <v>28</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13" s="16">
-        <v>205000</v>
-      </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="8">
-        <v>27</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="16">
-        <v>200000</v>
-      </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="8">
-        <v>26</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" s="16">
-        <v>200000</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="8">
-        <v>36</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" s="16">
-        <v>200000</v>
-      </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="8">
-        <v>28</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17" s="16">
-        <v>196267</v>
-      </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="12"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="8">
-        <v>26</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="16">
-        <v>196267</v>
-      </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="8">
-        <v>28</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F19" s="16">
-        <v>196267</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="8">
-        <v>30</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F20" s="16">
-        <v>196267</v>
-      </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="12"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="8">
-        <v>32</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="16">
-        <v>196267</v>
-      </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="8">
-        <v>35</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="16">
-        <v>196100</v>
-      </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="8">
-        <v>36</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="16">
-        <v>195000</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="8">
-        <v>33</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="16">
-        <v>195000</v>
-      </c>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="8">
-        <v>29</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="16">
-        <v>190550</v>
-      </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="12"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" s="8">
-        <v>32</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" s="16">
-        <v>190000</v>
-      </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="8">
-        <v>31</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" s="16">
-        <v>185400</v>
-      </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="12"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="8">
-        <v>29</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" s="16">
-        <v>185000</v>
-      </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="12"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="8">
-        <v>30</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29" s="16">
-        <v>185000</v>
-      </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="12"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="8">
-        <v>35</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="16">
-        <v>183000</v>
-      </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="8">
-        <v>27</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31" s="16">
-        <v>180250</v>
-      </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="12"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="8">
-        <v>26</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="16">
-        <v>170000</v>
-      </c>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="12"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="8">
-        <v>26</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" s="16">
-        <v>170000</v>
-      </c>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="8">
-        <v>27</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="16">
-        <v>164800</v>
-      </c>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="12"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="8">
-        <v>27</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F35" s="16">
-        <v>160000</v>
-      </c>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="12"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="8">
-        <v>29</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F36" s="16">
-        <v>160000</v>
-      </c>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="12"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="8">
-        <v>30</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F37" s="16">
-        <v>160000</v>
-      </c>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="12"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="8">
-        <v>28</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38" s="16">
-        <v>159000</v>
-      </c>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="12"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="8">
-        <v>33</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F39" s="16">
-        <v>155000</v>
-      </c>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="12"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="8">
-        <v>28</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F40" s="16">
-        <v>152800</v>
-      </c>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="12"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="8">
-        <v>34</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F41" s="16">
-        <v>150350</v>
-      </c>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="12"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="8">
-        <v>27</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" s="16">
-        <v>150000</v>
-      </c>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="8">
-        <v>27</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43" s="16">
-        <v>148400</v>
-      </c>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="12"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="8">
-        <v>32</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F44" s="16">
-        <v>145000</v>
-      </c>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="12"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="8">
-        <v>25</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F45" s="16">
-        <v>144000</v>
-      </c>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="12"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D46" s="8">
-        <v>29</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F46" s="16">
-        <v>141000</v>
-      </c>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="12"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="8">
-        <v>26</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F47" s="16">
-        <v>140000</v>
-      </c>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" s="8">
-        <v>35</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F48" s="16">
-        <v>140000</v>
-      </c>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="12"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" s="8">
-        <v>26</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F49" s="16">
-        <v>140000</v>
-      </c>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="12"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="8">
-        <v>28</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F50" s="16">
-        <v>139000</v>
-      </c>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="8">
-        <v>36</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F51" s="16">
-        <v>135000</v>
-      </c>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="12"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F51">
-    <sortCondition descending="1" ref="F2:F51"/>
-  </sortState>
-  <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>